<commit_message>
EDA + Model done
</commit_message>
<xml_diff>
--- a/BOVA11.xlsx
+++ b/BOVA11.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/154741817660f387/Projects/JupyterLabs/Analise/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gatar\Documents\GitHub\exploratory-data-analysis-bova11-etf-stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_F25DC773A252ABDACC1048D30919733A5ADE58EA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2D2C2F3B-0E2E-490E-B609-FF15960DEDBD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1045B9-FC4F-4A8E-B49C-E9A01777E4E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>CIA VALE DO RIO DOCE SH</t>
   </si>
   <si>
-    <t>Materiais</t>
-  </si>
-  <si>
     <t>BRVALEACNOR0</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>ITAU UNIBANCO HOLDING PREF SA</t>
   </si>
   <si>
-    <t>Produtos financeiros</t>
-  </si>
-  <si>
     <t>B037HR3</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>PETROLEO BRASILEIRO PREF SA</t>
   </si>
   <si>
-    <t>Energia</t>
-  </si>
-  <si>
     <t>BRPETRACNPR6</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>AMBEV SA</t>
   </si>
   <si>
-    <t>Bens de primeira necessidade</t>
-  </si>
-  <si>
     <t>BG7ZWY7</t>
   </si>
   <si>
@@ -186,9 +174,6 @@
     <t>WEG SA</t>
   </si>
   <si>
-    <t>Bens Industriais</t>
-  </si>
-  <si>
     <t>BRWEGEACNOR0</t>
   </si>
   <si>
@@ -399,9 +384,6 @@
     <t>TELEFONICA BRASIL PREF SA</t>
   </si>
   <si>
-    <t>Communication</t>
-  </si>
-  <si>
     <t>B3ZCNF7</t>
   </si>
   <si>
@@ -969,19 +951,37 @@
     <t>BRECORACNOR8</t>
   </si>
   <si>
-    <t>Consumo discricionario</t>
-  </si>
-  <si>
-    <t>Cuidados de saude</t>
-  </si>
-  <si>
-    <t>Imobiliario</t>
-  </si>
-  <si>
-    <t>Servicos publicos</t>
-  </si>
-  <si>
-    <t>Tecnologia de informacao</t>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>Real State</t>
+  </si>
+  <si>
+    <t>Telecom</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Public Services</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Consumer Staples</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>Consumer Discretionary</t>
   </si>
 </sst>
 </file>
@@ -1304,15 +1304,21 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1382,22 +1388,22 @@
         <v>1241817068.8</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I2">
         <v>2196286</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1405,10 +1411,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3">
         <v>6.33</v>
@@ -1426,22 +1432,22 @@
         <v>715106184</v>
       </c>
       <c r="H3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1449,10 +1455,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>5.16</v>
@@ -1470,22 +1476,22 @@
         <v>582760579.80999994</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1493,10 +1499,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>5.01</v>
@@ -1514,22 +1520,22 @@
         <v>566276020.20000005</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>314</v>
       </c>
       <c r="I5">
         <v>2684532</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1537,10 +1543,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>4.9000000000000004</v>
@@ -1558,22 +1564,22 @@
         <v>553566839.41999996</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1581,10 +1587,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>3.87</v>
@@ -1602,22 +1608,22 @@
         <v>437601392.25</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>314</v>
       </c>
       <c r="I7">
         <v>2682365</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1625,10 +1631,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8">
         <v>3.64</v>
@@ -1646,22 +1652,22 @@
         <v>411095582.30000001</v>
       </c>
       <c r="H8" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1669,10 +1675,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>3.28</v>
@@ -1690,22 +1696,22 @@
         <v>370142335.69</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1713,10 +1719,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>2.88</v>
@@ -1734,22 +1740,22 @@
         <v>324969172.30000001</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I10">
         <v>2945422</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1757,10 +1763,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>2.34</v>
@@ -1778,22 +1784,22 @@
         <v>264709046.16</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I11">
         <v>2458771</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1801,10 +1807,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>2.21</v>
@@ -1822,22 +1828,22 @@
         <v>249459230.08000001</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I12">
         <v>2328595</v>
       </c>
       <c r="J12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1845,10 +1851,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C13">
         <v>2.09</v>
@@ -1866,22 +1872,22 @@
         <v>235512205.5</v>
       </c>
       <c r="H13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -1889,10 +1895,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C14">
         <v>1.98</v>
@@ -1910,22 +1916,22 @@
         <v>223985968.5</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1933,10 +1939,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>1.97</v>
@@ -1954,22 +1960,22 @@
         <v>222242643.15000001</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1977,10 +1983,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>1.88</v>
@@ -1998,22 +2004,22 @@
         <v>211785088.31999999</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2021,10 +2027,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>1.71</v>
@@ -2042,22 +2048,22 @@
         <v>192877832.58000001</v>
       </c>
       <c r="H17" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2065,10 +2071,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C18">
         <v>1.68</v>
@@ -2086,22 +2092,22 @@
         <v>189634099.30000001</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2109,10 +2115,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C19">
         <v>1.67</v>
@@ -2130,22 +2136,22 @@
         <v>188873250.19</v>
       </c>
       <c r="H19" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -2153,10 +2159,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C20">
         <v>1.5</v>
@@ -2174,22 +2180,22 @@
         <v>169444114.5</v>
       </c>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -2197,10 +2203,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C21">
         <v>1.35</v>
@@ -2218,22 +2224,22 @@
         <v>152196920</v>
       </c>
       <c r="H21" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -2241,10 +2247,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C22">
         <v>1.33</v>
@@ -2262,22 +2268,22 @@
         <v>150370668.96000001</v>
       </c>
       <c r="H22" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -2285,10 +2291,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C23">
         <v>1.3</v>
@@ -2306,22 +2312,22 @@
         <v>146652655.19999999</v>
       </c>
       <c r="H23" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I23">
         <v>2683777</v>
       </c>
       <c r="J23" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -2329,10 +2335,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C24">
         <v>1.26</v>
@@ -2350,22 +2356,22 @@
         <v>142251811.19999999</v>
       </c>
       <c r="H24" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I24">
         <v>2516710</v>
       </c>
       <c r="J24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -2373,10 +2379,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C25">
         <v>1.2</v>
@@ -2394,22 +2400,22 @@
         <v>135974557</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I25">
         <v>2645517</v>
       </c>
       <c r="J25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -2417,10 +2423,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C26">
         <v>1.17</v>
@@ -2438,22 +2444,22 @@
         <v>132051168.40000001</v>
       </c>
       <c r="H26" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J26" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -2461,10 +2467,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C27">
         <v>1.1399999999999999</v>
@@ -2482,22 +2488,22 @@
         <v>128469573.7</v>
       </c>
       <c r="H27" t="s">
-        <v>32</v>
+        <v>314</v>
       </c>
       <c r="I27" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J27" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -2505,10 +2511,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C28">
         <v>1.03</v>
@@ -2526,22 +2532,22 @@
         <v>116098414.11</v>
       </c>
       <c r="H28" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I28" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J28" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -2549,10 +2555,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C29">
         <v>1.01</v>
@@ -2570,22 +2576,22 @@
         <v>114633118.2</v>
       </c>
       <c r="H29" t="s">
-        <v>123</v>
+        <v>309</v>
       </c>
       <c r="I29" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J29" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="K29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -2593,10 +2599,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C30">
         <v>0.96</v>
@@ -2614,22 +2620,22 @@
         <v>107868684.7</v>
       </c>
       <c r="H30" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I30" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J30" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="K30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N30">
         <v>1</v>
@@ -2637,10 +2643,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C31">
         <v>0.9</v>
@@ -2658,22 +2664,22 @@
         <v>101788975.2</v>
       </c>
       <c r="H31" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I31" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J31" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -2681,10 +2687,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C32">
         <v>0.86</v>
@@ -2702,22 +2708,22 @@
         <v>96618419.819999993</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I32" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J32" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -2725,10 +2731,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C33">
         <v>0.85</v>
@@ -2746,22 +2752,22 @@
         <v>96356933.75</v>
       </c>
       <c r="H33" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I33" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J33" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -2769,10 +2775,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C34">
         <v>0.79</v>
@@ -2790,22 +2796,22 @@
         <v>88764223.75</v>
       </c>
       <c r="H34" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I34">
         <v>2036995</v>
       </c>
       <c r="J34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="K34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -2813,10 +2819,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C35">
         <v>0.78</v>
@@ -2834,22 +2840,22 @@
         <v>88216324</v>
       </c>
       <c r="H35" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I35">
         <v>2840970</v>
       </c>
       <c r="J35" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N35">
         <v>1</v>
@@ -2857,10 +2863,10 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C36">
         <v>0.78</v>
@@ -2878,22 +2884,22 @@
         <v>87761443.680000007</v>
       </c>
       <c r="H36" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I36" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J36" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -2901,10 +2907,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C37">
         <v>0.72</v>
@@ -2922,22 +2928,22 @@
         <v>81207630</v>
       </c>
       <c r="H37" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="I37" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J37" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -2945,10 +2951,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C38">
         <v>0.7</v>
@@ -2966,22 +2972,22 @@
         <v>79374900.299999997</v>
       </c>
       <c r="H38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I38" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J38" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="K38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -2989,10 +2995,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C39">
         <v>0.63</v>
@@ -3010,22 +3016,22 @@
         <v>71454944.640000001</v>
       </c>
       <c r="H39" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I39" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J39" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -3033,10 +3039,10 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B40" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C40">
         <v>0.62</v>
@@ -3054,22 +3060,22 @@
         <v>70494414.540000007</v>
       </c>
       <c r="H40" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I40" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J40" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -3077,10 +3083,10 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C41">
         <v>0.62</v>
@@ -3098,22 +3104,22 @@
         <v>70163037</v>
       </c>
       <c r="H41" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I41" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J41" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N41">
         <v>1</v>
@@ -3121,10 +3127,10 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C42">
         <v>0.61</v>
@@ -3142,22 +3148,22 @@
         <v>69309122.079999998</v>
       </c>
       <c r="H42" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I42">
         <v>2311120</v>
       </c>
       <c r="J42" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -3165,10 +3171,10 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C43">
         <v>0.6</v>
@@ -3186,22 +3192,22 @@
         <v>68172208</v>
       </c>
       <c r="H43" t="s">
-        <v>123</v>
+        <v>309</v>
       </c>
       <c r="I43">
         <v>2292560</v>
       </c>
       <c r="J43" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="K43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N43">
         <v>1</v>
@@ -3209,10 +3215,10 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B44" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C44">
         <v>0.59</v>
@@ -3230,22 +3236,22 @@
         <v>66426143.850000001</v>
       </c>
       <c r="H44" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I44">
         <v>2667793</v>
       </c>
       <c r="J44" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="K44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -3253,10 +3259,10 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C45">
         <v>0.56999999999999995</v>
@@ -3274,22 +3280,22 @@
         <v>64909601.039999999</v>
       </c>
       <c r="H45" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I45" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="J45" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N45">
         <v>1</v>
@@ -3297,10 +3303,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C46">
         <v>0.56999999999999995</v>
@@ -3318,22 +3324,22 @@
         <v>64022390.520000003</v>
       </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I46" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J46" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -3341,10 +3347,10 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C47">
         <v>0.56000000000000005</v>
@@ -3362,22 +3368,22 @@
         <v>63672060.899999999</v>
       </c>
       <c r="H47" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I47" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J47" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="K47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -3385,10 +3391,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B48" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C48">
         <v>0.56000000000000005</v>
@@ -3406,22 +3412,22 @@
         <v>62722179.149999999</v>
       </c>
       <c r="H48" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I48" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J48" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -3429,10 +3435,10 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B49" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C49">
         <v>0.54</v>
@@ -3450,22 +3456,22 @@
         <v>60656400</v>
       </c>
       <c r="H49" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I49" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J49" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -3473,10 +3479,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B50" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C50">
         <v>0.5</v>
@@ -3494,22 +3500,22 @@
         <v>56414466.240000002</v>
       </c>
       <c r="H50" t="s">
-        <v>23</v>
+        <v>316</v>
       </c>
       <c r="I50" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="J50" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -3517,10 +3523,10 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C51">
         <v>0.5</v>
@@ -3538,22 +3544,22 @@
         <v>56143376.520000003</v>
       </c>
       <c r="H51" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I51" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="J51" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="K51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -3561,10 +3567,10 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C52">
         <v>0.48</v>
@@ -3582,22 +3588,22 @@
         <v>53648239.68</v>
       </c>
       <c r="H52" t="s">
-        <v>32</v>
+        <v>314</v>
       </c>
       <c r="I52" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="J52" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="K52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -3605,10 +3611,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B53" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C53">
         <v>0.47</v>
@@ -3626,22 +3632,22 @@
         <v>52743342.960000001</v>
       </c>
       <c r="H53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I53" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="J53" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -3649,10 +3655,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C54">
         <v>0.46</v>
@@ -3670,22 +3676,22 @@
         <v>51799574.200000003</v>
       </c>
       <c r="H54" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I54" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="J54" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="K54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -3693,10 +3699,10 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C55">
         <v>0.46</v>
@@ -3714,22 +3720,22 @@
         <v>51509080.979999997</v>
       </c>
       <c r="H55" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I55" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="J55" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="K55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -3737,10 +3743,10 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B56" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C56">
         <v>0.45</v>
@@ -3758,22 +3764,22 @@
         <v>51269242</v>
       </c>
       <c r="H56" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I56" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="J56" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="K56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -3781,10 +3787,10 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B57" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C57">
         <v>0.43</v>
@@ -3802,22 +3808,22 @@
         <v>48034214.280000001</v>
       </c>
       <c r="H57" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I57" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="J57" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="K57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -3825,10 +3831,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B58" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C58">
         <v>0.41</v>
@@ -3846,22 +3852,22 @@
         <v>46283712.740000002</v>
       </c>
       <c r="H58" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I58">
         <v>2308445</v>
       </c>
       <c r="J58" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="K58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -3869,10 +3875,10 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B59" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C59">
         <v>0.41</v>
@@ -3890,22 +3896,22 @@
         <v>46185023.329999998</v>
       </c>
       <c r="H59" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I59">
         <v>2189855</v>
       </c>
       <c r="J59" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="K59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -3913,10 +3919,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B60" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C60">
         <v>0.38</v>
@@ -3934,22 +3940,22 @@
         <v>42557916</v>
       </c>
       <c r="H60" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I60">
         <v>2648862</v>
       </c>
       <c r="J60" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -3957,10 +3963,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B61" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C61">
         <v>0.34</v>
@@ -3978,22 +3984,22 @@
         <v>38329592</v>
       </c>
       <c r="H61" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I61" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J61" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -4001,10 +4007,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B62" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C62">
         <v>0.33</v>
@@ -4022,22 +4028,22 @@
         <v>37099650</v>
       </c>
       <c r="H62" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I62" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J62" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="K62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -4045,10 +4051,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B63" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C63">
         <v>0.31</v>
@@ -4066,22 +4072,22 @@
         <v>35337089.840000004</v>
       </c>
       <c r="H63" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I63" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J63" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="K63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -4089,10 +4095,10 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B64" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C64">
         <v>0.3</v>
@@ -4110,22 +4116,22 @@
         <v>34133916.479999997</v>
       </c>
       <c r="H64" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I64" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="J64" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="K64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -4133,10 +4139,10 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B65" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C65">
         <v>0.28999999999999998</v>
@@ -4154,22 +4160,22 @@
         <v>32805166.600000001</v>
       </c>
       <c r="H65" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I65" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J65" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -4177,10 +4183,10 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B66" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C66">
         <v>0.28999999999999998</v>
@@ -4198,22 +4204,22 @@
         <v>32669167.960000001</v>
       </c>
       <c r="H66" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I66" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="J66" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="K66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L66" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -4221,10 +4227,10 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B67" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C67">
         <v>0.28999999999999998</v>
@@ -4242,22 +4248,22 @@
         <v>32564561.039999999</v>
       </c>
       <c r="H67" t="s">
-        <v>16</v>
+        <v>307</v>
       </c>
       <c r="I67">
         <v>2386009</v>
       </c>
       <c r="J67" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="K67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L67" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -4265,10 +4271,10 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B68" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C68">
         <v>0.28999999999999998</v>
@@ -4286,22 +4292,22 @@
         <v>32413139.190000001</v>
       </c>
       <c r="H68" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I68" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="J68" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="K68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L68" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N68">
         <v>1</v>
@@ -4309,10 +4315,10 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B69" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C69">
         <v>0.27</v>
@@ -4330,22 +4336,22 @@
         <v>30864984</v>
       </c>
       <c r="H69" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I69" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="J69" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="K69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -4353,10 +4359,10 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B70" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C70">
         <v>0.27</v>
@@ -4374,22 +4380,22 @@
         <v>30111143.239999998</v>
       </c>
       <c r="H70" t="s">
-        <v>32</v>
+        <v>314</v>
       </c>
       <c r="I70" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="J70" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -4397,10 +4403,10 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B71" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C71">
         <v>0.23</v>
@@ -4418,22 +4424,22 @@
         <v>25883742.5</v>
       </c>
       <c r="H71" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="I71" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="J71" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="K71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -4441,10 +4447,10 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B72" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C72">
         <v>0.2</v>
@@ -4462,22 +4468,22 @@
         <v>22615667.460000001</v>
       </c>
       <c r="H72" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I72" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="J72" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="K72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N72">
         <v>1</v>
@@ -4485,10 +4491,10 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B73" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C73">
         <v>0.16</v>
@@ -4506,22 +4512,22 @@
         <v>17898659.73</v>
       </c>
       <c r="H73" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="I73" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="J73" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="K73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L73" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -4529,10 +4535,10 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B74" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C74">
         <v>0.15</v>
@@ -4550,22 +4556,22 @@
         <v>17412570</v>
       </c>
       <c r="H74" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I74" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="J74" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="K74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L74" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -4573,10 +4579,10 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B75" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C75">
         <v>0.15</v>
@@ -4594,22 +4600,22 @@
         <v>16482910.08</v>
       </c>
       <c r="H75" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I75" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J75" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="K75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N75">
         <v>1</v>
@@ -4617,10 +4623,10 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B76" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C76">
         <v>0.13</v>
@@ -4638,22 +4644,22 @@
         <v>14527681.92</v>
       </c>
       <c r="H76" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I76" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="J76" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="K76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L76" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N76">
         <v>1</v>
@@ -4661,10 +4667,10 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B77" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C77">
         <v>0.12</v>
@@ -4682,22 +4688,22 @@
         <v>13909544</v>
       </c>
       <c r="H77" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="I77" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="J77" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="K77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N77">
         <v>1</v>
@@ -4705,10 +4711,10 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B78" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C78">
         <v>0.11</v>
@@ -4726,22 +4732,22 @@
         <v>12495613.9</v>
       </c>
       <c r="H78" t="s">
-        <v>52</v>
+        <v>313</v>
       </c>
       <c r="I78" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="J78" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="K78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N78">
         <v>1</v>

</xml_diff>